<commit_message>
Water chem and Respirometry update
</commit_message>
<xml_diff>
--- a/Broodstock_hemolymph_freezer_samples.xlsx
+++ b/Broodstock_hemolymph_freezer_samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/P_generosa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0A21B8-D38C-1347-8F4E-DBF9A97B3ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40EF46D-9573-DA46-BB56-7A1DF6C21785}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{71C09115-8CF9-A042-8DB2-38332BAD3ABC}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" activeTab="1" xr2:uid="{71C09115-8CF9-A042-8DB2-38332BAD3ABC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="161">
   <si>
     <t>animal</t>
   </si>
@@ -493,15 +493,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Nov 19 hemolymph</t>
-  </si>
-  <si>
-    <t>Dec 5 hemolymph</t>
-  </si>
-  <si>
-    <t>Jan 3 hemolHLmph</t>
   </si>
   <si>
     <t>HL</t>
@@ -570,12 +561,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578E305D-44F2-E747-B149-4335AE0CC8A6}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D142" sqref="A1:D142"/>
     </sheetView>
   </sheetViews>
@@ -2477,19 +2469,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{857E26E0-1642-074D-BD9E-1D3E9F834172}">
-  <dimension ref="A1:J142"/>
+  <dimension ref="A1:N142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2499,21 +2491,30 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D1">
+        <v>20190317</v>
+      </c>
+      <c r="E1">
+        <v>20190221</v>
+      </c>
+      <c r="F1">
+        <v>20190123</v>
+      </c>
+      <c r="G1" s="5">
+        <v>20190104</v>
+      </c>
+      <c r="H1">
+        <v>20181205</v>
+      </c>
+      <c r="I1">
+        <v>20181119</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2523,21 +2524,21 @@
       <c r="C2" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="N2" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2547,19 +2548,19 @@
       <c r="C3" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2569,19 +2570,22 @@
       <c r="C4" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2591,19 +2595,19 @@
       <c r="C5" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2613,19 +2617,19 @@
       <c r="C6" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2635,19 +2639,22 @@
       <c r="C7" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2657,19 +2664,19 @@
       <c r="C8" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2679,19 +2686,19 @@
       <c r="C9" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2701,19 +2708,19 @@
       <c r="C10" t="s">
         <v>150</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2723,19 +2730,19 @@
       <c r="C11" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2745,19 +2752,19 @@
       <c r="C12" t="s">
         <v>150</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2767,19 +2774,19 @@
       <c r="C13" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2789,19 +2796,22 @@
       <c r="C14" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2811,19 +2821,19 @@
       <c r="C15" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2833,19 +2843,19 @@
       <c r="C16" t="s">
         <v>150</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2855,19 +2865,22 @@
       <c r="C17" t="s">
         <v>150</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2877,19 +2890,19 @@
       <c r="C18" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2899,18 +2912,21 @@
       <c r="C19" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2920,18 +2936,18 @@
       <c r="C20" t="s">
         <v>150</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2941,18 +2957,18 @@
       <c r="C21" t="s">
         <v>150</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2962,18 +2978,18 @@
       <c r="C22" t="s">
         <v>150</v>
       </c>
-      <c r="D22" t="s">
-        <v>157</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>154</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2983,18 +2999,18 @@
       <c r="C23" t="s">
         <v>150</v>
       </c>
-      <c r="D23" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -3004,18 +3020,18 @@
       <c r="C24" t="s">
         <v>150</v>
       </c>
-      <c r="D24" t="s">
-        <v>157</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>154</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -3025,18 +3041,18 @@
       <c r="C25" t="s">
         <v>150</v>
       </c>
-      <c r="D25" t="s">
-        <v>146</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>146</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -3046,18 +3062,18 @@
       <c r="C26" t="s">
         <v>150</v>
       </c>
-      <c r="D26" t="s">
-        <v>157</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>154</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -3067,18 +3083,18 @@
       <c r="C27" t="s">
         <v>150</v>
       </c>
-      <c r="D27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -3088,18 +3104,18 @@
       <c r="C28" t="s">
         <v>150</v>
       </c>
-      <c r="D28" t="s">
-        <v>157</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -3109,18 +3125,18 @@
       <c r="C29" t="s">
         <v>150</v>
       </c>
-      <c r="D29" t="s">
-        <v>157</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>154</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -3130,18 +3146,18 @@
       <c r="C30" t="s">
         <v>150</v>
       </c>
-      <c r="D30" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>146</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -3151,18 +3167,18 @@
       <c r="C31" t="s">
         <v>150</v>
       </c>
-      <c r="D31" t="s">
-        <v>157</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>154</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -3172,18 +3188,18 @@
       <c r="C32" t="s">
         <v>150</v>
       </c>
-      <c r="D32" t="s">
-        <v>146</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>146</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -3193,18 +3209,18 @@
       <c r="C33" t="s">
         <v>150</v>
       </c>
-      <c r="D33" t="s">
-        <v>157</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -3214,18 +3230,18 @@
       <c r="C34" t="s">
         <v>150</v>
       </c>
-      <c r="D34" t="s">
-        <v>157</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -3235,18 +3251,18 @@
       <c r="C35" t="s">
         <v>150</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -3256,18 +3272,18 @@
       <c r="C36" t="s">
         <v>150</v>
       </c>
-      <c r="D36" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" t="s">
-        <v>146</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>146</v>
+      </c>
+      <c r="H36" t="s">
+        <v>146</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -3277,18 +3293,18 @@
       <c r="C37" t="s">
         <v>150</v>
       </c>
-      <c r="D37" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" t="s">
-        <v>146</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>146</v>
+      </c>
+      <c r="H37" t="s">
+        <v>146</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -3298,18 +3314,18 @@
       <c r="C38" t="s">
         <v>150</v>
       </c>
-      <c r="D38" t="s">
-        <v>157</v>
-      </c>
-      <c r="E38" t="s">
-        <v>153</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>154</v>
+      </c>
+      <c r="H38" t="s">
+        <v>153</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -3319,18 +3335,18 @@
       <c r="C39" t="s">
         <v>150</v>
       </c>
-      <c r="D39" t="s">
+      <c r="G39" t="s">
+        <v>154</v>
+      </c>
+      <c r="H39" t="s">
+        <v>153</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E39" t="s">
-        <v>153</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -3340,18 +3356,18 @@
       <c r="C40" t="s">
         <v>150</v>
       </c>
-      <c r="D40" t="s">
-        <v>157</v>
-      </c>
-      <c r="E40" t="s">
-        <v>153</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" t="s">
+        <v>153</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -3361,18 +3377,18 @@
       <c r="C41" t="s">
         <v>150</v>
       </c>
-      <c r="D41" t="s">
-        <v>157</v>
-      </c>
-      <c r="E41" t="s">
-        <v>153</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>154</v>
+      </c>
+      <c r="H41" t="s">
+        <v>153</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
@@ -3382,18 +3398,18 @@
       <c r="C42" t="s">
         <v>152</v>
       </c>
-      <c r="D42" t="s">
-        <v>157</v>
-      </c>
-      <c r="E42" t="s">
-        <v>153</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42" t="s">
+        <v>153</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>124</v>
       </c>
@@ -3403,18 +3419,18 @@
       <c r="C43" t="s">
         <v>152</v>
       </c>
-      <c r="D43" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" t="s">
-        <v>153</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>154</v>
+      </c>
+      <c r="H43" t="s">
+        <v>153</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>125</v>
       </c>
@@ -3424,18 +3440,18 @@
       <c r="C44" t="s">
         <v>152</v>
       </c>
-      <c r="D44" t="s">
-        <v>157</v>
-      </c>
-      <c r="E44" t="s">
-        <v>153</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>154</v>
+      </c>
+      <c r="H44" t="s">
+        <v>153</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>126</v>
       </c>
@@ -3445,18 +3461,18 @@
       <c r="C45" t="s">
         <v>152</v>
       </c>
-      <c r="D45" t="s">
-        <v>157</v>
-      </c>
-      <c r="E45" t="s">
-        <v>153</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45" t="s">
+        <v>153</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>127</v>
       </c>
@@ -3466,18 +3482,18 @@
       <c r="C46" t="s">
         <v>152</v>
       </c>
-      <c r="D46" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" t="s">
-        <v>153</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>154</v>
+      </c>
+      <c r="H46" t="s">
+        <v>153</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>128</v>
       </c>
@@ -3487,18 +3503,18 @@
       <c r="C47" t="s">
         <v>152</v>
       </c>
-      <c r="D47" t="s">
-        <v>157</v>
-      </c>
-      <c r="E47" t="s">
-        <v>153</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>154</v>
+      </c>
+      <c r="H47" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>129</v>
       </c>
@@ -3508,18 +3524,18 @@
       <c r="C48" t="s">
         <v>152</v>
       </c>
-      <c r="D48" t="s">
-        <v>157</v>
-      </c>
-      <c r="E48" t="s">
-        <v>153</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>154</v>
+      </c>
+      <c r="H48" t="s">
+        <v>153</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>130</v>
       </c>
@@ -3529,18 +3545,18 @@
       <c r="C49" t="s">
         <v>152</v>
       </c>
-      <c r="D49" t="s">
-        <v>157</v>
-      </c>
-      <c r="E49" t="s">
-        <v>153</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>154</v>
+      </c>
+      <c r="H49" t="s">
+        <v>153</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>131</v>
       </c>
@@ -3550,18 +3566,18 @@
       <c r="C50" t="s">
         <v>152</v>
       </c>
-      <c r="D50" t="s">
-        <v>157</v>
-      </c>
-      <c r="E50" t="s">
-        <v>153</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>154</v>
+      </c>
+      <c r="H50" t="s">
+        <v>153</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>132</v>
       </c>
@@ -3571,18 +3587,18 @@
       <c r="C51" t="s">
         <v>152</v>
       </c>
-      <c r="D51" t="s">
-        <v>157</v>
-      </c>
-      <c r="E51" t="s">
-        <v>153</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>154</v>
+      </c>
+      <c r="H51" t="s">
+        <v>153</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>133</v>
       </c>
@@ -3592,18 +3608,18 @@
       <c r="C52" t="s">
         <v>152</v>
       </c>
-      <c r="D52" t="s">
-        <v>157</v>
-      </c>
-      <c r="E52" t="s">
-        <v>153</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>154</v>
+      </c>
+      <c r="H52" t="s">
+        <v>153</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>134</v>
       </c>
@@ -3613,18 +3629,18 @@
       <c r="C53" t="s">
         <v>152</v>
       </c>
-      <c r="D53" t="s">
-        <v>157</v>
-      </c>
-      <c r="E53" t="s">
-        <v>153</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>154</v>
+      </c>
+      <c r="H53" t="s">
+        <v>153</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>135</v>
       </c>
@@ -3634,18 +3650,18 @@
       <c r="C54" t="s">
         <v>152</v>
       </c>
-      <c r="D54" t="s">
-        <v>157</v>
-      </c>
-      <c r="E54" t="s">
-        <v>153</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>154</v>
+      </c>
+      <c r="H54" t="s">
+        <v>153</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>136</v>
       </c>
@@ -3655,18 +3671,18 @@
       <c r="C55" t="s">
         <v>152</v>
       </c>
-      <c r="D55" t="s">
-        <v>157</v>
-      </c>
-      <c r="E55" t="s">
-        <v>153</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>154</v>
+      </c>
+      <c r="H55" t="s">
+        <v>153</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>137</v>
       </c>
@@ -3676,18 +3692,18 @@
       <c r="C56" t="s">
         <v>152</v>
       </c>
-      <c r="D56" t="s">
-        <v>157</v>
-      </c>
-      <c r="E56" t="s">
-        <v>153</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>154</v>
+      </c>
+      <c r="H56" t="s">
+        <v>153</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>138</v>
       </c>
@@ -3697,18 +3713,18 @@
       <c r="C57" t="s">
         <v>152</v>
       </c>
-      <c r="D57" t="s">
-        <v>157</v>
-      </c>
-      <c r="E57" t="s">
-        <v>153</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>154</v>
+      </c>
+      <c r="H57" t="s">
+        <v>153</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>139</v>
       </c>
@@ -3718,18 +3734,18 @@
       <c r="C58" t="s">
         <v>152</v>
       </c>
-      <c r="D58" t="s">
-        <v>157</v>
-      </c>
-      <c r="E58" t="s">
-        <v>153</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>154</v>
+      </c>
+      <c r="H58" t="s">
+        <v>153</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>140</v>
       </c>
@@ -3739,18 +3755,18 @@
       <c r="C59" t="s">
         <v>152</v>
       </c>
-      <c r="D59" t="s">
-        <v>157</v>
-      </c>
-      <c r="E59" t="s">
-        <v>153</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>154</v>
+      </c>
+      <c r="H59" t="s">
+        <v>153</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>141</v>
       </c>
@@ -3760,18 +3776,18 @@
       <c r="C60" t="s">
         <v>152</v>
       </c>
-      <c r="D60" t="s">
-        <v>146</v>
-      </c>
-      <c r="E60" t="s">
-        <v>146</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>146</v>
+      </c>
+      <c r="H60" t="s">
+        <v>146</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>142</v>
       </c>
@@ -3781,18 +3797,18 @@
       <c r="C61" t="s">
         <v>152</v>
       </c>
-      <c r="D61" t="s">
-        <v>146</v>
-      </c>
-      <c r="E61" t="s">
-        <v>146</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G61" t="s">
+        <v>146</v>
+      </c>
+      <c r="H61" t="s">
+        <v>146</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>43</v>
       </c>
@@ -3802,18 +3818,18 @@
       <c r="C62" t="s">
         <v>152</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G62" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>44</v>
       </c>
@@ -3823,18 +3839,18 @@
       <c r="C63" t="s">
         <v>152</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G63" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>45</v>
       </c>
@@ -3844,18 +3860,18 @@
       <c r="C64" t="s">
         <v>152</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G64" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>46</v>
       </c>
@@ -3865,18 +3881,18 @@
       <c r="C65" t="s">
         <v>152</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G65" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>47</v>
       </c>
@@ -3886,18 +3902,18 @@
       <c r="C66" t="s">
         <v>152</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G66" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>48</v>
       </c>
@@ -3907,18 +3923,18 @@
       <c r="C67" t="s">
         <v>152</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G67" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>49</v>
       </c>
@@ -3928,18 +3944,18 @@
       <c r="C68" t="s">
         <v>152</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G68" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>50</v>
       </c>
@@ -3949,18 +3965,18 @@
       <c r="C69" t="s">
         <v>152</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>51</v>
       </c>
@@ -3970,18 +3986,18 @@
       <c r="C70" t="s">
         <v>152</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G70" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>52</v>
       </c>
@@ -3991,18 +4007,18 @@
       <c r="C71" t="s">
         <v>152</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G71" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>53</v>
       </c>
@@ -4012,17 +4028,17 @@
       <c r="C72" t="s">
         <v>152</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G72" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>54</v>
       </c>
@@ -4032,17 +4048,17 @@
       <c r="C73" t="s">
         <v>152</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G73" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>55</v>
       </c>
@@ -4052,17 +4068,17 @@
       <c r="C74" t="s">
         <v>152</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G74" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>56</v>
       </c>
@@ -4072,17 +4088,17 @@
       <c r="C75" t="s">
         <v>152</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G75" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>57</v>
       </c>
@@ -4092,17 +4108,17 @@
       <c r="C76" t="s">
         <v>152</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G76" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>58</v>
       </c>
@@ -4112,17 +4128,17 @@
       <c r="C77" t="s">
         <v>152</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G77" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>59</v>
       </c>
@@ -4132,17 +4148,17 @@
       <c r="C78" t="s">
         <v>152</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G78" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>60</v>
       </c>
@@ -4152,17 +4168,17 @@
       <c r="C79" t="s">
         <v>152</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G79" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>61</v>
       </c>
@@ -4172,17 +4188,17 @@
       <c r="C80" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G80" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>62</v>
       </c>
@@ -4192,17 +4208,17 @@
       <c r="C81" t="s">
         <v>152</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G81" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>83</v>
       </c>
@@ -4212,18 +4228,18 @@
       <c r="C82" t="s">
         <v>151</v>
       </c>
-      <c r="D82" t="s">
-        <v>157</v>
-      </c>
-      <c r="E82" t="s">
-        <v>157</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G82" t="s">
+        <v>154</v>
+      </c>
+      <c r="H82" t="s">
+        <v>154</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
@@ -4233,18 +4249,18 @@
       <c r="C83" t="s">
         <v>151</v>
       </c>
-      <c r="D83" t="s">
-        <v>157</v>
-      </c>
-      <c r="E83" t="s">
-        <v>157</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G83" t="s">
+        <v>154</v>
+      </c>
+      <c r="H83" t="s">
+        <v>154</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
@@ -4254,18 +4270,18 @@
       <c r="C84" t="s">
         <v>151</v>
       </c>
-      <c r="D84" t="s">
-        <v>157</v>
-      </c>
-      <c r="E84" t="s">
-        <v>157</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G84" t="s">
+        <v>154</v>
+      </c>
+      <c r="H84" t="s">
+        <v>154</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>86</v>
       </c>
@@ -4275,18 +4291,18 @@
       <c r="C85" t="s">
         <v>151</v>
       </c>
-      <c r="D85" t="s">
-        <v>157</v>
-      </c>
-      <c r="E85" t="s">
-        <v>157</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G85" t="s">
+        <v>154</v>
+      </c>
+      <c r="H85" t="s">
+        <v>154</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
@@ -4296,18 +4312,18 @@
       <c r="C86" t="s">
         <v>151</v>
       </c>
-      <c r="D86" t="s">
-        <v>157</v>
-      </c>
-      <c r="E86" t="s">
-        <v>157</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G86" t="s">
+        <v>154</v>
+      </c>
+      <c r="H86" t="s">
+        <v>154</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>88</v>
       </c>
@@ -4317,18 +4333,18 @@
       <c r="C87" t="s">
         <v>151</v>
       </c>
-      <c r="D87" t="s">
-        <v>157</v>
-      </c>
-      <c r="E87" t="s">
-        <v>157</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G87" t="s">
+        <v>154</v>
+      </c>
+      <c r="H87" t="s">
+        <v>154</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>89</v>
       </c>
@@ -4338,18 +4354,18 @@
       <c r="C88" t="s">
         <v>151</v>
       </c>
-      <c r="D88" t="s">
-        <v>157</v>
-      </c>
-      <c r="E88" t="s">
-        <v>157</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G88" t="s">
+        <v>154</v>
+      </c>
+      <c r="H88" t="s">
+        <v>154</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>90</v>
       </c>
@@ -4359,18 +4375,18 @@
       <c r="C89" t="s">
         <v>151</v>
       </c>
-      <c r="D89" t="s">
-        <v>157</v>
-      </c>
-      <c r="E89" t="s">
-        <v>157</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G89" t="s">
+        <v>154</v>
+      </c>
+      <c r="H89" t="s">
+        <v>154</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>91</v>
       </c>
@@ -4380,18 +4396,18 @@
       <c r="C90" t="s">
         <v>151</v>
       </c>
-      <c r="D90" t="s">
-        <v>157</v>
-      </c>
-      <c r="E90" t="s">
-        <v>157</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G90" t="s">
+        <v>154</v>
+      </c>
+      <c r="H90" t="s">
+        <v>154</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
@@ -4401,18 +4417,18 @@
       <c r="C91" t="s">
         <v>151</v>
       </c>
-      <c r="D91" t="s">
-        <v>157</v>
-      </c>
-      <c r="E91" t="s">
-        <v>157</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G91" t="s">
+        <v>154</v>
+      </c>
+      <c r="H91" t="s">
+        <v>154</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>93</v>
       </c>
@@ -4422,18 +4438,18 @@
       <c r="C92" t="s">
         <v>151</v>
       </c>
-      <c r="D92" t="s">
-        <v>157</v>
-      </c>
-      <c r="E92" t="s">
-        <v>157</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G92" t="s">
+        <v>154</v>
+      </c>
+      <c r="H92" t="s">
+        <v>154</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>94</v>
       </c>
@@ -4443,18 +4459,18 @@
       <c r="C93" t="s">
         <v>151</v>
       </c>
-      <c r="D93" t="s">
-        <v>157</v>
-      </c>
-      <c r="E93" t="s">
-        <v>157</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G93" t="s">
+        <v>154</v>
+      </c>
+      <c r="H93" t="s">
+        <v>154</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>95</v>
       </c>
@@ -4464,18 +4480,18 @@
       <c r="C94" t="s">
         <v>151</v>
       </c>
-      <c r="D94" t="s">
-        <v>157</v>
-      </c>
-      <c r="E94" t="s">
-        <v>157</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G94" t="s">
+        <v>154</v>
+      </c>
+      <c r="H94" t="s">
+        <v>154</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>96</v>
       </c>
@@ -4485,18 +4501,18 @@
       <c r="C95" t="s">
         <v>151</v>
       </c>
-      <c r="D95" t="s">
-        <v>157</v>
-      </c>
-      <c r="E95" t="s">
-        <v>157</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G95" t="s">
+        <v>154</v>
+      </c>
+      <c r="H95" t="s">
+        <v>154</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>97</v>
       </c>
@@ -4506,18 +4522,18 @@
       <c r="C96" t="s">
         <v>151</v>
       </c>
-      <c r="D96" t="s">
-        <v>157</v>
-      </c>
-      <c r="E96" t="s">
-        <v>157</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G96" t="s">
+        <v>154</v>
+      </c>
+      <c r="H96" t="s">
+        <v>154</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>98</v>
       </c>
@@ -4527,18 +4543,18 @@
       <c r="C97" t="s">
         <v>151</v>
       </c>
-      <c r="D97" t="s">
-        <v>157</v>
-      </c>
-      <c r="E97" t="s">
-        <v>157</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>154</v>
+      </c>
+      <c r="H97" t="s">
+        <v>154</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>99</v>
       </c>
@@ -4548,18 +4564,18 @@
       <c r="C98" t="s">
         <v>151</v>
       </c>
-      <c r="D98" t="s">
-        <v>157</v>
-      </c>
-      <c r="E98" t="s">
-        <v>157</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G98" t="s">
+        <v>154</v>
+      </c>
+      <c r="H98" t="s">
+        <v>154</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>100</v>
       </c>
@@ -4569,18 +4585,18 @@
       <c r="C99" t="s">
         <v>151</v>
       </c>
-      <c r="D99" t="s">
-        <v>157</v>
-      </c>
-      <c r="E99" t="s">
-        <v>157</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G99" s="1"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G99" t="s">
+        <v>154</v>
+      </c>
+      <c r="H99" t="s">
+        <v>154</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>101</v>
       </c>
@@ -4590,18 +4606,18 @@
       <c r="C100" t="s">
         <v>151</v>
       </c>
-      <c r="D100" t="s">
-        <v>157</v>
-      </c>
-      <c r="E100" t="s">
-        <v>157</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G100" s="1"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G100" t="s">
+        <v>154</v>
+      </c>
+      <c r="H100" t="s">
+        <v>154</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J100" s="1"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>102</v>
       </c>
@@ -4611,18 +4627,18 @@
       <c r="C101" t="s">
         <v>151</v>
       </c>
-      <c r="D101" t="s">
-        <v>146</v>
-      </c>
-      <c r="E101" t="s">
-        <v>146</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G101" s="1"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G101" t="s">
+        <v>146</v>
+      </c>
+      <c r="H101" t="s">
+        <v>146</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>103</v>
       </c>
@@ -4632,18 +4648,18 @@
       <c r="C102" t="s">
         <v>152</v>
       </c>
-      <c r="D102" t="s">
-        <v>157</v>
-      </c>
-      <c r="E102" t="s">
-        <v>157</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G102" s="1"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G102" t="s">
+        <v>154</v>
+      </c>
+      <c r="H102" t="s">
+        <v>154</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>104</v>
       </c>
@@ -4653,18 +4669,18 @@
       <c r="C103" t="s">
         <v>152</v>
       </c>
-      <c r="D103" t="s">
-        <v>157</v>
-      </c>
-      <c r="E103" t="s">
-        <v>157</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G103" s="1"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G103" t="s">
+        <v>154</v>
+      </c>
+      <c r="H103" t="s">
+        <v>154</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>105</v>
       </c>
@@ -4674,18 +4690,18 @@
       <c r="C104" t="s">
         <v>152</v>
       </c>
-      <c r="D104" t="s">
-        <v>157</v>
-      </c>
-      <c r="E104" t="s">
-        <v>157</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G104" s="1"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G104" t="s">
+        <v>154</v>
+      </c>
+      <c r="H104" t="s">
+        <v>154</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>106</v>
       </c>
@@ -4695,18 +4711,18 @@
       <c r="C105" t="s">
         <v>152</v>
       </c>
-      <c r="D105" t="s">
-        <v>157</v>
-      </c>
-      <c r="E105" t="s">
-        <v>157</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G105" s="1"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G105" t="s">
+        <v>154</v>
+      </c>
+      <c r="H105" t="s">
+        <v>154</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>107</v>
       </c>
@@ -4716,18 +4732,18 @@
       <c r="C106" t="s">
         <v>152</v>
       </c>
-      <c r="D106" t="s">
-        <v>157</v>
-      </c>
-      <c r="E106" t="s">
-        <v>157</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G106" s="1"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G106" t="s">
+        <v>154</v>
+      </c>
+      <c r="H106" t="s">
+        <v>154</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J106" s="1"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>108</v>
       </c>
@@ -4737,18 +4753,18 @@
       <c r="C107" t="s">
         <v>152</v>
       </c>
-      <c r="D107" t="s">
-        <v>157</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G107" s="1"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G107" t="s">
+        <v>154</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>109</v>
       </c>
@@ -4758,18 +4774,18 @@
       <c r="C108" t="s">
         <v>152</v>
       </c>
-      <c r="D108" t="s">
-        <v>157</v>
-      </c>
-      <c r="E108" t="s">
-        <v>157</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G108" s="1"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G108" t="s">
+        <v>154</v>
+      </c>
+      <c r="H108" t="s">
+        <v>154</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>110</v>
       </c>
@@ -4779,18 +4795,18 @@
       <c r="C109" t="s">
         <v>152</v>
       </c>
-      <c r="D109" t="s">
-        <v>157</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G109" s="1"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G109" t="s">
+        <v>154</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>111</v>
       </c>
@@ -4800,18 +4816,18 @@
       <c r="C110" t="s">
         <v>152</v>
       </c>
-      <c r="D110" t="s">
-        <v>157</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G110" s="1"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G110" t="s">
+        <v>154</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J110" s="1"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>112</v>
       </c>
@@ -4821,18 +4837,18 @@
       <c r="C111" t="s">
         <v>152</v>
       </c>
-      <c r="D111" t="s">
-        <v>146</v>
-      </c>
-      <c r="E111" t="s">
-        <v>146</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G111" s="1"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G111" t="s">
+        <v>146</v>
+      </c>
+      <c r="H111" t="s">
+        <v>146</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J111" s="1"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>113</v>
       </c>
@@ -4842,18 +4858,18 @@
       <c r="C112" t="s">
         <v>152</v>
       </c>
-      <c r="D112" t="s">
-        <v>157</v>
-      </c>
-      <c r="E112" t="s">
-        <v>157</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G112" s="1"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G112" t="s">
+        <v>154</v>
+      </c>
+      <c r="H112" t="s">
+        <v>154</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J112" s="1"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>114</v>
       </c>
@@ -4863,18 +4879,18 @@
       <c r="C113" t="s">
         <v>152</v>
       </c>
-      <c r="D113" t="s">
-        <v>157</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G113" s="1"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G113" t="s">
+        <v>154</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J113" s="1"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>115</v>
       </c>
@@ -4884,18 +4900,18 @@
       <c r="C114" t="s">
         <v>152</v>
       </c>
-      <c r="D114" t="s">
-        <v>146</v>
-      </c>
-      <c r="E114" t="s">
-        <v>146</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G114" s="1"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G114" t="s">
+        <v>146</v>
+      </c>
+      <c r="H114" t="s">
+        <v>146</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J114" s="1"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>116</v>
       </c>
@@ -4905,18 +4921,18 @@
       <c r="C115" t="s">
         <v>152</v>
       </c>
-      <c r="D115" t="s">
-        <v>157</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G115" s="1"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G115" t="s">
+        <v>154</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J115" s="1"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>117</v>
       </c>
@@ -4926,18 +4942,18 @@
       <c r="C116" t="s">
         <v>152</v>
       </c>
-      <c r="D116" t="s">
-        <v>157</v>
-      </c>
-      <c r="E116" t="s">
-        <v>157</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G116" s="1"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G116" t="s">
+        <v>154</v>
+      </c>
+      <c r="H116" t="s">
+        <v>154</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J116" s="1"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>118</v>
       </c>
@@ -4947,18 +4963,18 @@
       <c r="C117" t="s">
         <v>152</v>
       </c>
-      <c r="D117" t="s">
-        <v>157</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G117" s="1"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G117" t="s">
+        <v>154</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>119</v>
       </c>
@@ -4968,18 +4984,18 @@
       <c r="C118" t="s">
         <v>152</v>
       </c>
-      <c r="D118" t="s">
-        <v>157</v>
-      </c>
-      <c r="E118" t="s">
-        <v>157</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G118" t="s">
+        <v>154</v>
+      </c>
+      <c r="H118" t="s">
+        <v>154</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J118" s="1"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>120</v>
       </c>
@@ -4989,18 +5005,18 @@
       <c r="C119" t="s">
         <v>152</v>
       </c>
-      <c r="D119" t="s">
-        <v>157</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G119" s="1"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G119" t="s">
+        <v>154</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J119" s="1"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>121</v>
       </c>
@@ -5010,18 +5026,18 @@
       <c r="C120" t="s">
         <v>152</v>
       </c>
-      <c r="D120" t="s">
-        <v>157</v>
-      </c>
-      <c r="E120" t="s">
-        <v>157</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G120" s="1"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G120" t="s">
+        <v>154</v>
+      </c>
+      <c r="H120" t="s">
+        <v>154</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J120" s="1"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>122</v>
       </c>
@@ -5031,18 +5047,18 @@
       <c r="C121" t="s">
         <v>152</v>
       </c>
-      <c r="D121" t="s">
-        <v>157</v>
-      </c>
-      <c r="E121" t="s">
-        <v>157</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G121" s="1"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G121" t="s">
+        <v>154</v>
+      </c>
+      <c r="H121" t="s">
+        <v>154</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J121" s="1"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>148</v>
       </c>
@@ -5052,33 +5068,33 @@
       <c r="C122" t="s">
         <v>152</v>
       </c>
-      <c r="D122" t="s">
-        <v>157</v>
-      </c>
-      <c r="E122" t="s">
-        <v>157</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G122" s="1"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G122" t="s">
+        <v>154</v>
+      </c>
+      <c r="H122" t="s">
+        <v>154</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J122" s="1"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
@@ -5124,7 +5140,7 @@
       <c r="A142" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H142">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K142">
     <sortCondition ref="B2:B142"/>
     <sortCondition ref="A2:A142"/>
   </sortState>

</xml_diff>